<commit_message>
fix the excel i think
</commit_message>
<xml_diff>
--- a/Documentation/Fiches Techniques/Classeur1.xlsx
+++ b/Documentation/Fiches Techniques/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Session 3\Projet-session-3\Documentation\Fiches Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC266BE-7354-4F73-A1A6-0D1C0D71C269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BE9873-6FE4-4304-B910-3312A87CB36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{795B4D18-003E-435D-BECD-9408242C1148}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>0 ANGLE</t>
   </si>
@@ -68,19 +68,31 @@
     <t>INPUT</t>
   </si>
   <si>
-    <t>~35</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>~ -20</t>
-  </si>
-  <si>
-    <t>~168</t>
-  </si>
-  <si>
     <t>~80</t>
+  </si>
+  <si>
+    <t>~165</t>
+  </si>
+  <si>
+    <t>~140</t>
+  </si>
+  <si>
+    <t>~255</t>
+  </si>
+  <si>
+    <t>~ -135</t>
+  </si>
+  <si>
+    <t>~-169</t>
+  </si>
+  <si>
+    <t>~169</t>
+  </si>
+  <si>
+    <t>~ 20</t>
   </si>
 </sst>
 </file>
@@ -110,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +132,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -145,6 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,278 +498,821 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322B12E8-024C-4558-833F-26D383C223D5}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="3" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="4">
         <v>0</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="4">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4">
         <v>50</v>
       </c>
-      <c r="D1">
+      <c r="E1" s="4">
         <v>93</v>
       </c>
-      <c r="E1">
+      <c r="F1" s="4">
         <v>95</v>
       </c>
-      <c r="F1">
+      <c r="G1" s="4">
         <v>105</v>
       </c>
-      <c r="G1">
+      <c r="H1" s="4">
         <v>110</v>
       </c>
-      <c r="H1">
+      <c r="I1" s="4">
         <v>115</v>
       </c>
-      <c r="I1">
+      <c r="J1" s="4">
         <v>120</v>
       </c>
-      <c r="J1">
+      <c r="K1" s="4">
         <v>135</v>
       </c>
-      <c r="K1">
+      <c r="L1" s="4">
         <v>142</v>
       </c>
-      <c r="L1">
+      <c r="M1" s="4">
         <v>147</v>
       </c>
-      <c r="M1">
+      <c r="N1" s="4">
         <v>160</v>
       </c>
-      <c r="N1">
+      <c r="O1" s="4">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
         <v>-90</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
+      <c r="E2">
+        <v>-10</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
         <v>45</v>
       </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2">
-        <v>90</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>90</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>315</v>
       </c>
-      <c r="C3">
-        <v>45</v>
-      </c>
       <c r="D3">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="E3">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F3">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="G3">
-        <v>45</v>
-      </c>
-      <c r="H3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3">
+        <v>135</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>171</v>
+      </c>
+      <c r="L3">
+        <v>180</v>
+      </c>
+      <c r="O3" t="s">
         <v>10</v>
       </c>
-      <c r="K3">
-        <v>180</v>
-      </c>
-      <c r="N3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>180</v>
+      </c>
+      <c r="F4">
+        <v>177</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>135</v>
+      </c>
+      <c r="L4">
         <v>95</v>
       </c>
-      <c r="E4">
-        <v>183</v>
-      </c>
-      <c r="I4">
-        <v>135</v>
-      </c>
-      <c r="K4">
-        <v>85</v>
-      </c>
-      <c r="L4">
-        <v>90</v>
+      <c r="M4">
+        <v>90</v>
+      </c>
+      <c r="N4">
+        <v>62</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="E5">
-        <v>180</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="F5">
+        <v>180</v>
+      </c>
+      <c r="O5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>6</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2">
+        <v>30</v>
+      </c>
+      <c r="F14" s="2">
+        <v>40</v>
+      </c>
+      <c r="G14" s="2">
+        <v>50</v>
+      </c>
+      <c r="H14" s="2">
+        <v>60</v>
+      </c>
+      <c r="I14" s="2">
+        <v>70</v>
+      </c>
+      <c r="J14" s="2">
+        <v>80</v>
+      </c>
+      <c r="K14" s="2">
+        <v>90</v>
+      </c>
+      <c r="L14" s="2">
+        <v>100</v>
+      </c>
+      <c r="M14" s="2">
+        <v>110</v>
+      </c>
+      <c r="N14" s="2">
+        <v>120</v>
+      </c>
+      <c r="O14" s="2">
+        <v>130</v>
+      </c>
+      <c r="P14" s="2">
+        <v>140</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>150</v>
+      </c>
+      <c r="R14" s="2">
+        <v>160</v>
+      </c>
+      <c r="S14" s="2">
+        <v>170</v>
+      </c>
+      <c r="T14" s="2">
+        <v>180</v>
+      </c>
+      <c r="U14" s="2">
+        <v>190</v>
+      </c>
+      <c r="V14" s="2">
+        <v>200</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B15" s="3">
+        <v>-169</v>
+      </c>
+      <c r="C15" s="3">
+        <v>-151</v>
+      </c>
+      <c r="D15" s="3">
+        <v>-133</v>
+      </c>
+      <c r="E15" s="3">
+        <v>-115</v>
+      </c>
+      <c r="F15" s="3">
+        <v>-97</v>
+      </c>
+      <c r="G15" s="3">
+        <v>-90</v>
+      </c>
+      <c r="H15" s="3">
+        <v>-70</v>
+      </c>
+      <c r="I15" s="3">
+        <v>-50</v>
+      </c>
+      <c r="J15" s="3">
+        <v>-30</v>
+      </c>
+      <c r="K15" s="3">
+        <v>-10</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>10</v>
+      </c>
+      <c r="N15" s="3">
+        <v>45</v>
+      </c>
+      <c r="O15" s="3">
+        <v>62</v>
+      </c>
+      <c r="P15" s="3">
+        <v>80</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>85</v>
+      </c>
+      <c r="R15" s="3">
+        <v>90</v>
+      </c>
+      <c r="S15" s="3">
+        <v>110</v>
+      </c>
+      <c r="T15" s="3">
+        <v>130</v>
+      </c>
+      <c r="U15" s="3">
+        <v>150</v>
+      </c>
+      <c r="V15" s="3">
+        <v>169</v>
+      </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="3">
+        <v>315</v>
+      </c>
+      <c r="C16" s="3">
+        <v>333</v>
+      </c>
+      <c r="D16" s="3">
+        <v>351</v>
+      </c>
+      <c r="E16" s="3">
+        <v>23</v>
+      </c>
+      <c r="F16" s="3">
+        <v>32</v>
+      </c>
+      <c r="G16" s="3">
+        <v>90</v>
+      </c>
+      <c r="H16" s="3">
+        <v>113</v>
+      </c>
+      <c r="I16" s="3">
+        <v>126</v>
+      </c>
+      <c r="J16" s="3">
+        <v>139</v>
+      </c>
+      <c r="K16" s="3">
+        <v>152</v>
+      </c>
+      <c r="L16" s="3">
+        <v>135</v>
+      </c>
+      <c r="M16" s="3">
+        <v>140</v>
+      </c>
+      <c r="N16" s="3">
+        <v>171</v>
+      </c>
+      <c r="O16" s="3">
+        <v>176</v>
+      </c>
+      <c r="P16" s="3">
+        <v>180</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>180</v>
+      </c>
+      <c r="R16" s="3">
+        <v>180</v>
+      </c>
+      <c r="S16" s="3">
+        <v>180</v>
+      </c>
+      <c r="T16" s="3">
+        <v>180</v>
+      </c>
+      <c r="U16" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3">
+        <v>180</v>
+      </c>
+      <c r="L17" s="3">
+        <v>171</v>
+      </c>
+      <c r="M17" s="3">
+        <v>165</v>
+      </c>
+      <c r="N17" s="3">
+        <v>150</v>
+      </c>
+      <c r="O17" s="3">
+        <v>142</v>
+      </c>
+      <c r="P17" s="3">
+        <v>135</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>112</v>
+      </c>
+      <c r="R17" s="3">
+        <v>90</v>
+      </c>
+      <c r="S17" s="3">
+        <v>90</v>
+      </c>
+      <c r="T17" s="3">
+        <v>90</v>
+      </c>
+      <c r="U17" s="3">
+        <v>90</v>
+      </c>
+      <c r="V17" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
         <v>10</v>
       </c>
+      <c r="D22" s="2">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2">
+        <v>25</v>
+      </c>
+      <c r="F22" s="2">
+        <v>30</v>
+      </c>
+      <c r="G22" s="2">
+        <v>40</v>
+      </c>
+      <c r="H22" s="2">
+        <v>50</v>
+      </c>
+      <c r="I22" s="2">
+        <v>60</v>
+      </c>
+      <c r="J22" s="2">
+        <v>70</v>
+      </c>
+      <c r="K22" s="2">
+        <v>80</v>
+      </c>
+      <c r="L22" s="2">
+        <v>90</v>
+      </c>
+      <c r="M22" s="2">
+        <v>93</v>
+      </c>
+      <c r="N22" s="2">
+        <v>95</v>
+      </c>
+      <c r="O22" s="2">
+        <v>100</v>
+      </c>
+      <c r="P22" s="2">
+        <v>105</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>110</v>
+      </c>
+      <c r="R22" s="2">
+        <v>115</v>
+      </c>
+      <c r="S22" s="2">
+        <v>120</v>
+      </c>
+      <c r="T22" s="2">
+        <v>130</v>
+      </c>
+      <c r="U22" s="2">
+        <v>135</v>
+      </c>
+      <c r="V22" s="2">
+        <v>140</v>
+      </c>
+      <c r="W22" s="2">
+        <v>142</v>
+      </c>
+      <c r="X22" s="2">
+        <v>147</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>150</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>160</v>
+      </c>
+      <c r="AA22" s="2">
+        <v>170</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>180</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>190</v>
+      </c>
+      <c r="AD22" s="2">
+        <v>200</v>
+      </c>
+      <c r="AE22" s="2">
+        <v>205</v>
+      </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>20</v>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="3">
+        <v>-169</v>
+      </c>
+      <c r="C23" s="3">
+        <v>-157</v>
+      </c>
+      <c r="D23" s="3">
+        <v>-145</v>
+      </c>
+      <c r="E23" s="3">
+        <v>-135</v>
+      </c>
+      <c r="F23" s="3">
+        <v>-123</v>
+      </c>
+      <c r="G23" s="3">
+        <v>-107</v>
+      </c>
+      <c r="H23" s="3">
+        <v>-90</v>
+      </c>
+      <c r="I23" s="3">
+        <v>-77</v>
+      </c>
+      <c r="J23" s="3">
+        <v>-64</v>
+      </c>
+      <c r="K23" s="3">
+        <v>-51</v>
+      </c>
+      <c r="L23" s="3">
+        <v>-38</v>
+      </c>
+      <c r="M23" s="3">
+        <v>-10</v>
+      </c>
+      <c r="N23" s="3">
+        <v>-8</v>
+      </c>
+      <c r="O23" s="3">
+        <v>-4</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>7</v>
+      </c>
+      <c r="R23" s="3">
+        <v>14</v>
+      </c>
+      <c r="S23" s="3">
+        <v>45</v>
+      </c>
+      <c r="T23" s="3">
+        <v>56</v>
+      </c>
+      <c r="U23" s="3">
+        <v>67</v>
+      </c>
+      <c r="V23" s="3">
+        <v>74</v>
+      </c>
+      <c r="W23" s="3">
+        <v>77</v>
+      </c>
+      <c r="X23" s="3">
+        <v>83</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>87</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>90</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>100</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>115</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>130</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>150</v>
+      </c>
+      <c r="AE23" s="3">
+        <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>30</v>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3">
+        <v>315</v>
+      </c>
+      <c r="C24" s="3">
+        <v>324</v>
+      </c>
+      <c r="D24" s="3">
+        <v>333</v>
+      </c>
+      <c r="E24" s="3">
+        <v>41</v>
+      </c>
+      <c r="F24" s="3">
+        <v>58</v>
+      </c>
+      <c r="G24" s="3">
+        <v>74</v>
+      </c>
+      <c r="H24" s="3">
+        <v>90</v>
+      </c>
+      <c r="I24" s="3">
+        <v>92</v>
+      </c>
+      <c r="J24" s="3">
+        <v>94</v>
+      </c>
+      <c r="K24" s="3">
+        <v>95</v>
+      </c>
+      <c r="L24" s="3">
+        <v>95</v>
+      </c>
+      <c r="M24" s="3">
+        <v>95</v>
+      </c>
+      <c r="N24" s="3">
+        <v>116</v>
+      </c>
+      <c r="O24" s="3">
+        <v>126</v>
+      </c>
+      <c r="P24" s="3">
+        <v>135</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>138</v>
+      </c>
+      <c r="R24" s="3">
+        <v>145</v>
+      </c>
+      <c r="S24" s="3">
+        <v>171</v>
+      </c>
+      <c r="T24" s="3">
+        <v>176</v>
+      </c>
+      <c r="U24" s="3">
+        <v>180</v>
+      </c>
+      <c r="V24" s="3">
+        <v>180</v>
+      </c>
+      <c r="W24" s="3">
+        <v>180</v>
+      </c>
+      <c r="X24" s="3">
+        <v>180</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>180</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>180</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>180</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>180</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>180</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>255</v>
+      </c>
+      <c r="C25" s="3">
+        <v>247</v>
+      </c>
+      <c r="D25" s="3">
+        <v>239</v>
+      </c>
+      <c r="E25" s="3">
+        <v>235</v>
+      </c>
+      <c r="F25" s="3">
+        <v>231</v>
+      </c>
+      <c r="G25" s="3">
+        <v>223</v>
+      </c>
+      <c r="H25" s="3">
+        <v>215</v>
+      </c>
+      <c r="I25" s="3">
+        <v>207</v>
+      </c>
+      <c r="J25" s="3">
+        <v>199</v>
+      </c>
+      <c r="K25" s="3">
+        <v>190</v>
+      </c>
+      <c r="L25" s="3">
+        <v>182</v>
+      </c>
+      <c r="M25" s="3">
+        <v>180</v>
+      </c>
+      <c r="N25" s="3">
+        <v>177</v>
+      </c>
+      <c r="O25" s="3">
+        <v>171</v>
+      </c>
+      <c r="P25" s="3">
+        <v>165</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>160</v>
+      </c>
+      <c r="R25" s="3">
+        <v>155</v>
+      </c>
+      <c r="S25" s="3">
+        <v>150</v>
+      </c>
+      <c r="T25" s="3">
+        <v>140</v>
+      </c>
+      <c r="U25" s="3">
         <v>135</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3">
-        <v>170</v>
+      <c r="V25" s="3">
+        <v>115</v>
+      </c>
+      <c r="W25" s="3">
+        <v>95</v>
+      </c>
+      <c r="X25" s="3">
+        <v>90</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>88</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>83</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>78</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>73</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>67</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>62</v>
+      </c>
+      <c r="AE25" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remade half of the arm function but its now cleaner and easyer to use
</commit_message>
<xml_diff>
--- a/Documentation/Fiches Techniques/Classeur1.xlsx
+++ b/Documentation/Fiches Techniques/Classeur1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Session 3\Projet-session-3\Documentation\Fiches Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733543DD-CCCC-4194-A1FA-3EFCFF1FEF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F3BF3C-1239-4663-A539-0712E09BA57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{795B4D18-003E-435D-BECD-9408242C1148}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{795B4D18-003E-435D-BECD-9408242C1148}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>0 ANGLE</t>
   </si>
@@ -56,12 +56,6 @@
     <t>4 ANGLE</t>
   </si>
   <si>
-    <t>ouvert</t>
-  </si>
-  <si>
-    <t>fermé</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -114,6 +108,15 @@
   </si>
   <si>
     <t xml:space="preserve">distance (cm, ignoring height) from base to pivot 2 </t>
+  </si>
+  <si>
+    <t>0 Deg = open</t>
+  </si>
+  <si>
+    <t>90 Deg = closed</t>
+  </si>
+  <si>
+    <t>Angle-4</t>
   </si>
 </sst>
 </file>
@@ -182,20 +185,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,17 +536,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322B12E8-024C-4558-833F-26D383C223D5}">
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
     <col min="16" max="16" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -602,10 +606,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>-90</v>
@@ -617,19 +621,19 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L2">
         <v>45</v>
       </c>
       <c r="N2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O2">
         <v>90</v>
       </c>
       <c r="P2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -637,13 +641,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>120</v>
@@ -670,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -690,7 +694,7 @@
         <v>180</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I4">
         <v>213</v>
@@ -741,35 +745,61 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" t="s">
-        <v>7</v>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>24</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>55</v>
+      </c>
+      <c r="K6">
+        <v>61</v>
+      </c>
+      <c r="L6">
+        <v>64</v>
+      </c>
+      <c r="P6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>23</v>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="8">
         <v>0</v>
       </c>
       <c r="B13" s="3">
@@ -781,12 +811,15 @@
       <c r="D13" s="3">
         <v>34</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>327</v>
       </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="8">
         <v>10</v>
       </c>
       <c r="B14" s="3">
@@ -798,12 +831,15 @@
       <c r="D14" s="3">
         <v>49</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>308</v>
       </c>
+      <c r="F14" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="8">
         <v>20</v>
       </c>
       <c r="B15" s="3">
@@ -815,12 +851,15 @@
       <c r="D15" s="3">
         <v>64</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <v>298</v>
       </c>
+      <c r="F15" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="8">
         <v>25</v>
       </c>
       <c r="B16" s="3">
@@ -832,12 +871,15 @@
       <c r="D16" s="3">
         <v>72</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <v>288</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="F16" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
         <v>30</v>
       </c>
       <c r="B17" s="3">
@@ -849,12 +891,15 @@
       <c r="D17" s="3">
         <v>80</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>279</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="F17" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
         <v>40</v>
       </c>
       <c r="B18" s="3">
@@ -866,12 +911,15 @@
       <c r="D18" s="3">
         <v>95</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <v>260</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="F18" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
         <v>50</v>
       </c>
       <c r="B19" s="3">
@@ -883,12 +931,15 @@
       <c r="D19" s="3">
         <v>110</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>249</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="F19" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
         <v>60</v>
       </c>
       <c r="B20" s="3">
@@ -900,12 +951,15 @@
       <c r="D20" s="3">
         <v>127</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <v>234</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="F20" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
         <v>70</v>
       </c>
       <c r="B21" s="3">
@@ -917,12 +971,15 @@
       <c r="D21" s="3">
         <v>144</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <v>221</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="F21" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
         <v>75</v>
       </c>
       <c r="B22" s="3">
@@ -934,12 +991,15 @@
       <c r="D22" s="3">
         <v>152</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <v>209</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="F22" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
         <v>80</v>
       </c>
       <c r="B23" s="3">
@@ -951,12 +1011,15 @@
       <c r="D23" s="3">
         <v>160</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>204</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="F23" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
         <v>90</v>
       </c>
       <c r="B24" s="3">
@@ -968,12 +1031,15 @@
       <c r="D24" s="3">
         <v>175</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <v>192</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="F24" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
         <v>93</v>
       </c>
       <c r="B25" s="3">
@@ -985,12 +1051,15 @@
       <c r="D25" s="3">
         <v>180</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>187</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="F25" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
         <v>95</v>
       </c>
       <c r="B26" s="3">
@@ -1002,12 +1071,15 @@
       <c r="D26" s="3">
         <v>183</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="5">
         <v>180</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="F26" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
         <v>100</v>
       </c>
       <c r="B27" s="3">
@@ -1019,12 +1091,15 @@
       <c r="D27" s="3">
         <v>193</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="5">
         <v>168</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="F27" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
         <v>105</v>
       </c>
       <c r="B28" s="3">
@@ -1036,12 +1111,15 @@
       <c r="D28" s="3">
         <v>203</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="5">
         <v>160</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="F28" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
         <v>110</v>
       </c>
       <c r="B29" s="3">
@@ -1053,12 +1131,15 @@
       <c r="D29" s="3">
         <v>213</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="5">
         <v>152</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="F29" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
         <v>115</v>
       </c>
       <c r="B30" s="3">
@@ -1070,12 +1151,15 @@
       <c r="D30" s="3">
         <v>221</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="5">
         <v>144</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+      <c r="F30" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
         <v>120</v>
       </c>
       <c r="B31" s="3">
@@ -1087,12 +1171,15 @@
       <c r="D31" s="3">
         <v>232</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="5">
         <v>135</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
+      <c r="F31" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
         <v>130</v>
       </c>
       <c r="B32" s="3">
@@ -1104,12 +1191,15 @@
       <c r="D32" s="3">
         <v>249</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="5">
         <v>122</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
+      <c r="F32" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
         <v>135</v>
       </c>
       <c r="B33" s="3">
@@ -1121,12 +1211,15 @@
       <c r="D33" s="3">
         <v>257</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="5">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+      <c r="F33" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
         <v>140</v>
       </c>
       <c r="B34" s="3">
@@ -1138,12 +1231,15 @@
       <c r="D34" s="3">
         <v>267</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="5">
         <v>104</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
+      <c r="F34" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
         <v>142</v>
       </c>
       <c r="B35" s="3">
@@ -1155,12 +1251,15 @@
       <c r="D35" s="3">
         <v>270</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="5">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="3">
+      <c r="F35" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
         <v>147</v>
       </c>
       <c r="B36" s="3">
@@ -1172,12 +1271,15 @@
       <c r="D36" s="3">
         <v>277</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="5">
         <v>90</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
+      <c r="F36" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
         <v>150</v>
       </c>
       <c r="B37" s="3">
@@ -1189,12 +1291,15 @@
       <c r="D37" s="3">
         <v>282</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="5">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="3">
+      <c r="F37" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
         <v>160</v>
       </c>
       <c r="B38" s="3">
@@ -1206,12 +1311,15 @@
       <c r="D38" s="3">
         <v>299</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="5">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="3">
+      <c r="F38" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
         <v>170</v>
       </c>
       <c r="B39" s="3">
@@ -1223,12 +1331,15 @@
       <c r="D39" s="3">
         <v>316</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="5">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
+      <c r="F39" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
         <v>180</v>
       </c>
       <c r="B40" s="3">
@@ -1240,12 +1351,15 @@
       <c r="D40" s="3">
         <v>333</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="5">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
+      <c r="F40" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
         <v>190</v>
       </c>
       <c r="B41" s="3">
@@ -1257,12 +1371,15 @@
       <c r="D41" s="3">
         <v>350</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="5">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="3">
+      <c r="F41" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
         <v>200</v>
       </c>
       <c r="B42" s="3">
@@ -1274,12 +1391,15 @@
       <c r="D42" s="3">
         <v>367</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="3">
+      <c r="F42" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
         <v>205</v>
       </c>
       <c r="B43" s="3">
@@ -1291,16 +1411,19 @@
       <c r="D43" s="3">
         <v>375</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="5">
         <v>25</v>
       </c>
+      <c r="F43" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="59" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>22</v>
+      <c r="A59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1375,26 +1498,26 @@
       </c>
     </row>
     <row r="76" spans="1:2" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>24</v>
+      <c r="A76" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="7">
+      <c r="A77" s="5">
         <v>15</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="5">
         <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="7">
+      <c r="A78" s="5">
         <v>17</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B78" s="5">
         <v>20</v>
       </c>
     </row>
@@ -1407,10 +1530,10 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="7">
+      <c r="A80" s="5">
         <v>22</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B80" s="5">
         <v>30</v>
       </c>
     </row>

</xml_diff>